<commit_message>
11/30 Automation Log Program
</commit_message>
<xml_diff>
--- a/Documents/DebtPlan11_05_20.xlsx
+++ b/Documents/DebtPlan11_05_20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CodeBase\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46965D7A-AA8D-4F89-88CC-F3E7E6ADF6C8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB71ACA-3AFF-4D8A-9B1B-B43B01C04089}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,15 +78,6 @@
     <t>School Payment</t>
   </si>
   <si>
-    <t>Paycheck+Sick</t>
-  </si>
-  <si>
-    <t>Paycheck+Taxes</t>
-  </si>
-  <si>
-    <t>Paycheck+Tuition</t>
-  </si>
-  <si>
     <t>Anticipated Expenses</t>
   </si>
   <si>
@@ -100,6 +91,15 @@
   </si>
   <si>
     <t>3rd Paycheck</t>
+  </si>
+  <si>
+    <t>Sick</t>
+  </si>
+  <si>
+    <t>Taxes</t>
+  </si>
+  <si>
+    <t>Cards</t>
   </si>
 </sst>
 </file>
@@ -995,7 +995,7 @@
   <dimension ref="C1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L33" sqref="L32:L33"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1140,7 @@
         <v>3500</v>
       </c>
       <c r="H7" s="6">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="I7" s="8">
         <v>400</v>
@@ -1152,11 +1152,11 @@
       <c r="L7" s="2"/>
       <c r="M7" s="19">
         <f>D7+H7-I7-J7-K7+M6</f>
-        <v>0</v>
+        <v>-200</v>
       </c>
       <c r="N7" s="20">
         <f>M7-F7-G7</f>
-        <v>-4450</v>
+        <v>-4650</v>
       </c>
     </row>
     <row r="8" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1164,14 +1164,14 @@
         <v>44169</v>
       </c>
       <c r="D8" s="18">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="0"/>
-        <v>750</v>
+        <v>950</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" si="1"/>
@@ -1181,7 +1181,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="8">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="J8" s="8">
         <v>0</v>
@@ -1190,11 +1190,11 @@
       <c r="L8" s="2"/>
       <c r="M8" s="19">
         <f>D8+H8-I8-J8-K8+M7</f>
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N8" s="20">
         <f t="shared" ref="N8:N19" si="2">M8-F8-G8</f>
-        <v>-4250</v>
+        <v>-3650</v>
       </c>
     </row>
     <row r="9" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1202,14 +1202,14 @@
         <v>44183</v>
       </c>
       <c r="D9" s="18">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="0"/>
-        <v>750</v>
+        <v>950</v>
       </c>
       <c r="G9" s="7">
         <f t="shared" si="1"/>
@@ -1232,11 +1232,11 @@
       </c>
       <c r="M9" s="19">
         <f t="shared" ref="M9:M19" si="3">D9+H9-I9-J9-K9+M8</f>
-        <v>-400</v>
+        <v>200</v>
       </c>
       <c r="N9" s="20">
         <f t="shared" si="2"/>
-        <v>-4650</v>
+        <v>-4250</v>
       </c>
     </row>
     <row r="10" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1247,7 +1247,7 @@
         <v>700</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="0"/>
@@ -1261,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="8">
-        <v>750</v>
+        <v>950</v>
       </c>
       <c r="J10" s="8">
         <v>0</v>
@@ -1270,11 +1270,11 @@
       <c r="L10" s="2"/>
       <c r="M10" s="19">
         <f t="shared" si="3"/>
-        <v>-450</v>
+        <v>-50</v>
       </c>
       <c r="N10" s="20">
         <f t="shared" si="2"/>
-        <v>-3950</v>
+        <v>-3550</v>
       </c>
     </row>
     <row r="11" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1282,10 +1282,10 @@
         <v>44211</v>
       </c>
       <c r="D11" s="18">
-        <v>900</v>
+        <v>500</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="0"/>
@@ -1358,10 +1358,10 @@
         <v>44239</v>
       </c>
       <c r="D13" s="18">
-        <v>3600</v>
+        <v>3400</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="0"/>
@@ -1369,7 +1369,7 @@
       </c>
       <c r="G13" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="H13" s="6">
         <v>0</v>
@@ -1378,17 +1378,17 @@
         <v>0</v>
       </c>
       <c r="J13" s="8">
-        <v>3500</v>
+        <v>0</v>
       </c>
       <c r="K13" s="8"/>
       <c r="L13" s="2"/>
       <c r="M13" s="19">
         <f t="shared" si="3"/>
-        <v>750</v>
+        <v>4050</v>
       </c>
       <c r="N13" s="20">
         <f t="shared" si="2"/>
-        <v>750</v>
+        <v>550</v>
       </c>
     </row>
     <row r="14" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1407,7 +1407,7 @@
       </c>
       <c r="G14" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="H14" s="6">
         <v>0</v>
@@ -1424,11 +1424,11 @@
       <c r="L14" s="2"/>
       <c r="M14" s="19">
         <f t="shared" si="3"/>
-        <v>950</v>
+        <v>4250</v>
       </c>
       <c r="N14" s="20">
         <f t="shared" si="2"/>
-        <v>950</v>
+        <v>750</v>
       </c>
     </row>
     <row r="15" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="G15" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="H15" s="6">
         <v>0</v>
@@ -1462,11 +1462,11 @@
       <c r="L15" s="2"/>
       <c r="M15" s="19">
         <f t="shared" si="3"/>
-        <v>1150</v>
+        <v>4450</v>
       </c>
       <c r="N15" s="20">
         <f t="shared" si="2"/>
-        <v>1150</v>
+        <v>950</v>
       </c>
     </row>
     <row r="16" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="G16" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="H16" s="6">
         <v>0</v>
@@ -1500,11 +1500,11 @@
       <c r="L16" s="2"/>
       <c r="M16" s="19">
         <f t="shared" si="3"/>
-        <v>1350</v>
+        <v>4650</v>
       </c>
       <c r="N16" s="20">
         <f t="shared" si="2"/>
-        <v>1350</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="17" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="G17" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="H17" s="6">
         <v>0</v>
@@ -1538,11 +1538,11 @@
       <c r="L17" s="2"/>
       <c r="M17" s="19">
         <f t="shared" si="3"/>
-        <v>1550</v>
+        <v>4850</v>
       </c>
       <c r="N17" s="20">
         <f t="shared" si="2"/>
-        <v>1550</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="18" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="G18" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="H18" s="6">
         <v>0</v>
@@ -1576,11 +1576,11 @@
       <c r="L18" s="2"/>
       <c r="M18" s="19">
         <f t="shared" si="3"/>
-        <v>1750</v>
+        <v>5050</v>
       </c>
       <c r="N18" s="20">
         <f t="shared" si="2"/>
-        <v>1750</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="19" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="G19" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="H19" s="6">
         <v>0</v>
@@ -1614,11 +1614,11 @@
       <c r="L19" s="2"/>
       <c r="M19" s="19">
         <f t="shared" si="3"/>
-        <v>1950</v>
+        <v>5250</v>
       </c>
       <c r="N19" s="20">
         <f t="shared" si="2"/>
-        <v>1950</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="20" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1707,20 +1707,20 @@
     </row>
     <row r="27" spans="3:14" ht="19.5" x14ac:dyDescent="0.3">
       <c r="D27" s="28" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E27" s="28"/>
       <c r="F27" s="28"/>
     </row>
     <row r="28" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D28" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>6</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.25">
@@ -1760,7 +1760,7 @@
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D36" s="16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E36" s="16"/>
       <c r="F36" s="17">

</xml_diff>